<commit_message>
working on run 648
</commit_message>
<xml_diff>
--- a/library/library_0641.xlsx
+++ b/library/library_0641.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E735B3-17E2-B544-A673-66B55D873117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9625E5A3-89EC-F64F-A3B0-CC6090DBDE48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="12280" windowHeight="10800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,13 +176,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,7 +498,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="B3:B19 E2:E19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -510,33 +507,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -558,11 +555,11 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -584,11 +581,11 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -610,11 +607,11 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -636,11 +633,11 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -662,11 +659,11 @@
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -688,11 +685,11 @@
       <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -714,11 +711,11 @@
       <c r="G8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -740,11 +737,11 @@
       <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -766,11 +763,11 @@
       <c r="G10" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -792,11 +789,11 @@
       <c r="G11" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -818,11 +815,11 @@
       <c r="G12" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -844,11 +841,11 @@
       <c r="G13" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -870,11 +867,11 @@
       <c r="G14" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -896,11 +893,11 @@
       <c r="G15" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -922,11 +919,11 @@
       <c r="G16" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -948,11 +945,11 @@
       <c r="G17" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -974,11 +971,11 @@
       <c r="G18" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +997,7 @@
       <c r="G19" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>